<commit_message>
Restricting for only pairs indicatd
</commit_message>
<xml_diff>
--- a/Inputs/idef.xlsx
+++ b/Inputs/idef.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://idbg-my.sharepoint.com/personal/dcor_iadb_org/Documents/Documents/GitHub/calculo_indicators_R/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{0394DCB6-EA5C-432F-AAA9-0634268ADF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C80BB8C6-B681-412A-AFC2-F0BA5C502203}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:40009_{0394DCB6-EA5C-432F-AAA9-0634268ADF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{780D013D-E7AA-4CCD-B2BF-D1F273271B39}"/>
   <bookViews>
-    <workbookView xWindow="21900" yWindow="1260" windowWidth="14400" windowHeight="7440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34320" yWindow="3600" windowWidth="19185" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="idef" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>indicator_name</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>sex,ethnicity,area,isoalpha3,year</t>
+  </si>
+  <si>
+    <t>ethnicity,disability,migrante,area</t>
   </si>
 </sst>
 </file>
@@ -917,12 +920,12 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -942,7 +945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -959,10 +962,10 @@
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -982,7 +985,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>

</xml_diff>